<commit_message>
adaptando plano de aula
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,96 +13,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Data</t>
   </si>
   <si>
-    <t>Questão/Problema/Desafio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fundamentos / Conteúdo</t>
+    <t>Questão</t>
+  </si>
+  <si>
+    <t>Conteúdo</t>
   </si>
   <si>
     <t xml:space="preserve">Evidências de Aprendizado</t>
   </si>
   <si>
-    <t>Programação/Atividades</t>
-  </si>
-  <si>
-    <t>14-Ago</t>
-  </si>
-  <si>
-    <t>16-Ago</t>
-  </si>
-  <si>
-    <t>21-Ago</t>
-  </si>
-  <si>
-    <t>23-Ago</t>
-  </si>
-  <si>
-    <t>28-Ago</t>
-  </si>
-  <si>
-    <t>30-Ago</t>
+    <t>Atividades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O que é empreender?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empreendedorismo para a vida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empreendedorismo é um comportamento para o desenvolvimento de pessoas, de organizações e do mundo; Aproveite as oportunidades que serão oferecidas no curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação da disciplina; Bate papo com empreendedores do Insper.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O que é empreender em IA?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impactos atuais e futuros da IA; Visão geral das startups de IA; Projetos de pesquisa promissores de IA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como entender a situação atual e futura da IA e suas aplicações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-aula: pesquisa de startups de IA no Crunchbase e outras referências;  Desafio das startups mais promissoras; Desafio dos projetos de IA mais promissores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento de startups na visão dos investidores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entendimento da lógica de investimento de venture capital; Aprendendo a relacionar-se com investidores.</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>04-Set</t>
-  </si>
-  <si>
-    <t>06-Set</t>
-  </si>
-  <si>
-    <t>11-Set</t>
-  </si>
-  <si>
-    <t>13-Set</t>
-  </si>
-  <si>
-    <t>18-Set</t>
-  </si>
-  <si>
-    <t>20-Set</t>
-  </si>
-  <si>
-    <t>25-Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEMANA DE PROVAS</t>
-  </si>
-  <si>
-    <t>27-Set</t>
-  </si>
-  <si>
-    <t>02-Out</t>
-  </si>
-  <si>
-    <t>04-Out</t>
-  </si>
-  <si>
-    <t>09-Out</t>
-  </si>
-  <si>
-    <t>11-Out</t>
-  </si>
-  <si>
-    <t>16-Out</t>
-  </si>
-  <si>
-    <t>18-Out</t>
-  </si>
-  <si>
-    <t>23-Out</t>
-  </si>
-  <si>
-    <t>25-Out</t>
-  </si>
-  <si>
-    <t>30-Out</t>
+    <t>&lt;strong&gt;4&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Café com VC: Happy hour com investidores com teses de investimento em AI&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Expansão de networking; Entendimento das teses de investimento dos VCs.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Encontro informal com investidores convidados.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lições aprendidas com os investidores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansão do networking. Entendimento das teses de investimento dos VCs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debate sobre os aprendizados durante happy hour com investidores.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;6&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Breakfest @ Corps: Café da Manhã com as corporações com demandas de AI.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Expansão do networking. Entendimento das demandas das corporações que podem ser solucionadas com AI.&lt;/strong&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Encontro informal com executivos de inovação das corporações.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lições aprendidas com as corporações. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansão do networking. Entendimento das demandas das corporações que podem ser solucionadas com AI.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debate sobre os aprendizados durante o café da manhã com executivos de inovação das corporações. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O que é impactado pela sua solução?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição de oportunidades para empreender.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificação de oportunidades. Formação de equipes com capacidades complementares.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré-aula: descrição de problema que pode ser resolvido com IA. Dinâmica para apresentação e seleção de problemas. Dinâmica de formação de equipes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento do lean canvas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Compreensão do tamanho a oportunidade. Melhor entendimento do problema. Melhor definição da solução. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Preparação do pitch problem-solution-opportunity</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;11&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Apresentação do pitch Problem-Solution-Opportunity para investidores e corporações.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Compreensão do tamanho a oportunidade. Melhor entendimento do problema. Melhor definição da solução. &lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Pitch para investidores mais feedbacks.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lições aprendidas com o pitch para investidores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão do tamanho da oportunidade. Revisão do entendimento do problema. Revisão da solução. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debate sobre os aprendizados a partir do pitch para investidores. Revisão do lean canvas da oportunidade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como desenvolver soluções de IA?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A solução imaginada é factível? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRISP-DM ou KDD ou reutilização de modelos ou serviços</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infra-estrutura (github, nuvem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testes automatizados</t>
   </si>
 </sst>
 </file>
@@ -150,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -164,10 +224,7 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -681,15 +738,15 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="19.147857142857141"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="38.862142857142857"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="65.290714285714287"/>
+    <col customWidth="1" min="2" max="2" style="1" width="26.28125"/>
+    <col customWidth="1" min="3" max="3" style="1" width="31.00390625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="85.719285714285704"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="120.7192857142857"/>
     <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="13.005000000000001"/>
@@ -714,206 +771,280 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
+      <c r="A4" s="4">
+        <v>3</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
+    <row r="5" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
+      <c r="A6" s="3">
+        <v>5</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="63.75" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="47.25" customHeight="1">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>22</v>
+      <c r="A17" s="4">
+        <v>16</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>23</v>
+      <c r="A18" s="3">
+        <v>17</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A19" s="4" t="s">
-        <v>24</v>
+      <c r="A19" s="3">
+        <v>18</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>25</v>
+      <c r="A20" s="4">
+        <v>19</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -922,8 +1053,8 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="56.25" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>26</v>
+      <c r="A21" s="3">
+        <v>20</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -932,8 +1063,8 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
+      <c r="A22" s="3">
+        <v>21</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -942,8 +1073,8 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>28</v>
+      <c r="A23" s="3">
+        <v>22</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -952,8 +1083,8 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>29</v>
+      <c r="A24" s="4">
+        <v>23</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -962,8 +1093,8 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="5">
-        <v>45231</v>
+      <c r="A25" s="3">
+        <v>24</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -972,8 +1103,8 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="6">
-        <v>45236</v>
+      <c r="A26" s="3">
+        <v>25</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -982,8 +1113,8 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="6">
-        <v>45238</v>
+      <c r="A27" s="4">
+        <v>26</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -992,8 +1123,8 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="6">
-        <v>45243</v>
+      <c r="A28" s="3">
+        <v>27</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1002,7 +1133,9 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1010,7 +1143,9 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1018,7 +1153,9 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1026,7 +1163,9 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="2"/>
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1034,7 +1173,9 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="2"/>
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1042,7 +1183,9 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="2"/>
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1050,7 +1193,9 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="2"/>
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1058,12 +1203,29 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="1"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
plano de aula mais métodos de avaliacao
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Data</t>
   </si>
@@ -60,42 +60,45 @@
     <t xml:space="preserve">Entendimento da lógica de investimento de venture capital; Aprendendo a relacionar-se com investidores.</t>
   </si>
   <si>
+    <t xml:space="preserve">Debate com os estudantes sobre desenvolvimento de startups na visão dos investidores.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;4&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Café com VC: Happy hour com investidores com teses de investimento em AI&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Expansão de networking; Entendimento das teses de investimento dos VCs.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Encontro informal com investidores convidados.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lições aprendidas com os investidores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansão do networking. Entendimento das teses de investimento dos VCs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debate sobre os aprendizados durante happy hour com investidores.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;6&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Breakfest @ Corps: Café da Manhã com as corporações com demandas de AI.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Expansão do networking. Entendimento das demandas das corporações que podem ser solucionadas com AI.&lt;/strong&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Encontro informal com executivos de inovação das corporações.&lt;/strong&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>&lt;strong&gt;4&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Café com VC: Happy hour com investidores com teses de investimento em AI&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Expansão de networking; Entendimento das teses de investimento dos VCs.&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Encontro informal com investidores convidados.&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lições aprendidas com os investidores.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expansão do networking. Entendimento das teses de investimento dos VCs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debate sobre os aprendizados durante happy hour com investidores.</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;6&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Breakfest @ Corps: Café da Manhã com as corporações com demandas de AI.&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Expansão do networking. Entendimento das demandas das corporações que podem ser solucionadas com AI.&lt;/strong&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Encontro informal com executivos de inovação das corporações.&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lições aprendidas com as corporações. </t>
   </si>
   <si>
@@ -150,19 +153,109 @@
     <t xml:space="preserve">Como desenvolver soluções de IA?</t>
   </si>
   <si>
-    <t xml:space="preserve">A solução imaginada é factível? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRISP-DM ou KDD ou reutilização de modelos ou serviços</t>
-  </si>
-  <si>
-    <t>MVP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infra-estrutura (github, nuvem)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testes automatizados</t>
+    <t xml:space="preserve">A solução imaginada é factível? Quais são os recursos necessários para o desenvolvimento da solução? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapeamento modelo, fontes de informação e dados. Mapeamento da qualidade e disponibilidade dos dados. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercício que envolve a identificação das informações necessárias para o desenvolvimento da solução, mapeamento das fontes disponíveis de dados, da qualidade destas fontes e real disponibilidade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual o processo normalmente empregado no desenvolvimento de soluções de machine learning? CRISP-DM, KDD e reutilização de modelos e serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRISP-DM, KDD, identificação de oportunidades para reutilização de modelos e utilização de serviços de IA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva sobre os processos normalmente empregados no mercado e debate sobre como aplicar tais processos no desenvolvimento da solução de cada equipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produto Viável Mínimo (MVP). Por que usar este conceito? Como definir o seu MVP? A importância de um roadmap para a solução.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição do MVP para cada solução. Elaboração inicial de um roadmap.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breve exposição sobre o conceito de MVP seguido por debate sobre a definição dos MVPs para cada solução. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infra-estrutura (github, nuvem). Processos de trabalho (branch, pull request)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infra-estutura do projeto configurada e processos de trabalho definidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debate sobre o uso de github, serviços em nuvem e processos de trabalho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processos, MVP, infra-estrutura na prática</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As equipes souberam definir o seu MVP? Fizeram o mapeamento de dados necessários? Estão com a infra-estrutura configurada?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkpoint com todas as equipes para verificar os artefatos de projeto produzidos até o momento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testes automatizados, documentação e padronização de código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada equipe deverá definir como os testes automatizados, documentação e padronização de código serão feitos no escopo dos seus projetos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breve exposição sobre a importância de testes automatizados, documentação e padronização de código no escopo de startups. Apresentação de ferramentas que podem auxiliar as equipes nestas tarefas. Discussão entre as equipes para definir os padrões e ferramentas que serão adotados em cada equipe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento da solução</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evolução do código gerado, do quadro de atividades, dos modelos de machine learning e das funcionalidades da solução.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento da solução.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 1&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint review&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Apresentação e debate sobre as entregas do sprint.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 2&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 3&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 4&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 5&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Demo day&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Apresentação das soluções para a comunidade externa&lt;/strong&gt;</t>
   </si>
 </sst>
 </file>
@@ -210,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -226,6 +319,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +834,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -869,7 +965,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
@@ -878,13 +974,13 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -893,16 +989,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -912,13 +1008,13 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -928,29 +1024,29 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="50.25" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -960,13 +1056,13 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -975,35 +1071,49 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="41.25" customHeight="1">
+    <row r="15" s="1" customFormat="1" ht="78.75" customHeight="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="47.25" customHeight="1">
+    <row r="16" s="1" customFormat="1" ht="63.75" customHeight="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -1012,10 +1122,14 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="41.25" customHeight="1">
@@ -1023,11 +1137,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="41.25" customHeight="1">
@@ -1036,20 +1154,32 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="49.5" customHeight="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="56.25" customHeight="1">
@@ -1057,9 +1187,15 @@
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="44.25" customHeight="1">
@@ -1067,9 +1203,15 @@
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="34.5" customHeight="1">
@@ -1077,9 +1219,15 @@
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="37.5" customHeight="1">
@@ -1087,9 +1235,15 @@
         <v>23</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1097,9 +1251,15 @@
         <v>24</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1107,9 +1267,15 @@
         <v>25</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1117,9 +1283,15 @@
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1127,9 +1299,15 @@
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1137,9 +1315,15 @@
         <v>28</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1147,9 +1331,15 @@
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1157,9 +1347,15 @@
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1167,9 +1363,15 @@
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1177,9 +1379,15 @@
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1187,9 +1395,15 @@
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1197,9 +1411,15 @@
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="C35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="18" customHeight="1">
@@ -1207,24 +1427,71 @@
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" ht="28.5">
       <c r="A37" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" ht="14.25">
+      <c r="C37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" ht="28.5">
       <c r="A38" s="5">
         <v>37</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="5">
         <v>38</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alteracao pós comentários Nakagawa
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Data</t>
   </si>
@@ -30,6 +30,9 @@
     <t>Atividades</t>
   </si>
   <si>
+    <t xml:space="preserve">Atividade prévia</t>
+  </si>
+  <si>
     <t xml:space="preserve">O que é empreender?</t>
   </si>
   <si>
@@ -127,6 +130,15 @@
   </si>
   <si>
     <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Preparação do pitch problem-solution-opportunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento do lean canvas + Pitch para Investidores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Compreensão do tamanho a oportunidade. Melhor entendimento do problema. Melhor definição da solução. E transformação desses aprendizados em uma apresentação para investidores (Pitch para Investidores)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Preparação do pitch problem-solution-opportunity. E início da elaboração do Pitch para Investidores. </t>
   </si>
   <si>
     <t>&lt;strong&gt;11&lt;/strong&gt;</t>
@@ -311,6 +323,9 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -319,9 +334,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,7 +846,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -845,7 +857,7 @@
     <col customWidth="1" min="3" max="3" style="1" width="31.00390625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="85.719285714285704"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="120.7192857142857"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="13.005000000000001"/>
+    <col customWidth="1" min="6" max="6" style="1" width="17.00390625"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="18" customHeight="1">
@@ -864,561 +876,563 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>63</v>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A20" s="4">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>67</v>
+      <c r="B20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="56.25" customHeight="1">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>67</v>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>67</v>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="3">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
+      <c r="E28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="3">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="3">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="4">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="3">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="3">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>70</v>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -1428,70 +1442,70 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" ht="28.5">
-      <c r="A37" s="5">
+      <c r="A37" s="6">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="38" ht="28.5">
-      <c r="A38" s="5">
+      <c r="A38" s="6">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="5">
+      <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>70</v>
+      <c r="C39" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="5">
+      <c r="A40" s="6">
         <v>39</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>80</v>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste programacao levando-se em consideracao calendario 2024
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Data</t>
   </si>
@@ -33,6 +33,9 @@
     <t xml:space="preserve">Atividade prévia</t>
   </si>
   <si>
+    <t>6-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">O que é empreender?</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t xml:space="preserve">Apresentação da disciplina; Bate papo com empreendedores do Insper.</t>
   </si>
   <si>
+    <t>8-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">O que é empreender em IA?</t>
   </si>
   <si>
@@ -57,6 +63,15 @@
     <t xml:space="preserve">Pré-aula: pesquisa de startups de IA no Crunchbase e outras referências;  Desafio das startups mais promissoras; Desafio dos projetos de IA mais promissores.</t>
   </si>
   <si>
+    <t>13-Fev</t>
+  </si>
+  <si>
+    <t>Carnaval</t>
+  </si>
+  <si>
+    <t>15-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolvimento de startups na visão dos investidores</t>
   </si>
   <si>
@@ -66,7 +81,7 @@
     <t xml:space="preserve">Debate com os estudantes sobre desenvolvimento de startups na visão dos investidores.</t>
   </si>
   <si>
-    <t>&lt;strong&gt;4&lt;/strong&gt;</t>
+    <t>&lt;strong&gt;20-Fev&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Café com VC: Happy hour com investidores com teses de investimento em AI&lt;/strong&gt;</t>
@@ -78,6 +93,9 @@
     <t xml:space="preserve">&lt;strong&gt;Encontro informal com investidores convidados.&lt;/strong&gt;</t>
   </si>
   <si>
+    <t>22-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lições aprendidas com os investidores.</t>
   </si>
   <si>
@@ -87,7 +105,7 @@
     <t xml:space="preserve">Debate sobre os aprendizados durante happy hour com investidores.</t>
   </si>
   <si>
-    <t>&lt;strong&gt;6&lt;/strong&gt;</t>
+    <t>&lt;strong&gt;27-Fev&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Breakfest @ Corps: Café da Manhã com as corporações com demandas de AI.&lt;/strong&gt;</t>
@@ -102,6 +120,9 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
+    <t>29-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lições aprendidas com as corporações. </t>
   </si>
   <si>
@@ -111,6 +132,9 @@
     <t xml:space="preserve">Debate sobre os aprendizados durante o café da manhã com executivos de inovação das corporações. </t>
   </si>
   <si>
+    <t>05-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">O que é impactado pela sua solução?</t>
   </si>
   <si>
@@ -123,6 +147,9 @@
     <t xml:space="preserve">Pré-aula: descrição de problema que pode ser resolvido com IA. Dinâmica para apresentação e seleção de problemas. Dinâmica de formação de equipes.</t>
   </si>
   <si>
+    <t>07-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolvimento do lean canvas.</t>
   </si>
   <si>
@@ -132,6 +159,9 @@
     <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Preparação do pitch problem-solution-opportunity</t>
   </si>
   <si>
+    <t>12-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolvimento do lean canvas + Pitch para Investidores</t>
   </si>
   <si>
@@ -141,7 +171,7 @@
     <t xml:space="preserve">Desenvolvimento conceitual da solução, métricas, clientes entre outros componentes do lean canvas. Preparação do pitch problem-solution-opportunity. E início da elaboração do Pitch para Investidores. </t>
   </si>
   <si>
-    <t>&lt;strong&gt;11&lt;/strong&gt;</t>
+    <t>&lt;strong&gt;14-Março&lt;/strong&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Apresentação do pitch Problem-Solution-Opportunity para investidores e corporações.&lt;/strong&gt;</t>
@@ -153,6 +183,9 @@
     <t xml:space="preserve">&lt;strong&gt;Pitch para investidores mais feedbacks.&lt;/strong&gt;</t>
   </si>
   <si>
+    <t>19-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lições aprendidas com o pitch para investidores</t>
   </si>
   <si>
@@ -162,6 +195,9 @@
     <t xml:space="preserve">Debate sobre os aprendizados a partir do pitch para investidores. Revisão do lean canvas da oportunidade. </t>
   </si>
   <si>
+    <t>21-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como desenvolver soluções de IA?</t>
   </si>
   <si>
@@ -174,6 +210,9 @@
     <t xml:space="preserve">Exercício que envolve a identificação das informações necessárias para o desenvolvimento da solução, mapeamento das fontes disponíveis de dados, da qualidade destas fontes e real disponibilidade. </t>
   </si>
   <si>
+    <t>26-Março</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qual o processo normalmente empregado no desenvolvimento de soluções de machine learning? CRISP-DM, KDD e reutilização de modelos e serviços</t>
   </si>
   <si>
@@ -183,6 +222,18 @@
     <t xml:space="preserve">Aula expositiva sobre os processos normalmente empregados no mercado e debate sobre como aplicar tais processos no desenvolvimento da solução de cada equipe</t>
   </si>
   <si>
+    <t>28-Março</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação intermediária - não teremos aula</t>
+  </si>
+  <si>
+    <t>02-Abril</t>
+  </si>
+  <si>
+    <t>04-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Produto Viável Mínimo (MVP). Por que usar este conceito? Como definir o seu MVP? A importância de um roadmap para a solução.</t>
   </si>
   <si>
@@ -192,6 +243,9 @@
     <t xml:space="preserve">Breve exposição sobre o conceito de MVP seguido por debate sobre a definição dos MVPs para cada solução. </t>
   </si>
   <si>
+    <t>09-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Infra-estrutura (github, nuvem). Processos de trabalho (branch, pull request)</t>
   </si>
   <si>
@@ -201,6 +255,9 @@
     <t xml:space="preserve">Debate sobre o uso de github, serviços em nuvem e processos de trabalho.</t>
   </si>
   <si>
+    <t>11-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Processos, MVP, infra-estrutura na prática</t>
   </si>
   <si>
@@ -210,6 +267,9 @@
     <t xml:space="preserve">Checkpoint com todas as equipes para verificar os artefatos de projeto produzidos até o momento.</t>
   </si>
   <si>
+    <t>16-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testes automatizados, documentação e padronização de código</t>
   </si>
   <si>
@@ -219,6 +279,9 @@
     <t xml:space="preserve">Breve exposição sobre a importância de testes automatizados, documentação e padronização de código no escopo de startups. Apresentação de ferramentas que podem auxiliar as equipes nestas tarefas. Discussão entre as equipes para definir os padrões e ferramentas que serão adotados em cada equipe. </t>
   </si>
   <si>
+    <t>18-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolvimento da solução</t>
   </si>
   <si>
@@ -231,6 +294,15 @@
     <t xml:space="preserve">Desenvolvimento da solução.</t>
   </si>
   <si>
+    <t>23-Abril</t>
+  </si>
+  <si>
+    <t>25-Abril</t>
+  </si>
+  <si>
+    <t>30-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;Sprint 1&lt;/strong&gt;</t>
   </si>
   <si>
@@ -240,28 +312,49 @@
     <t xml:space="preserve">&lt;strong&gt;Apresentação e debate sobre as entregas do sprint.&lt;/strong&gt;</t>
   </si>
   <si>
+    <t>02-Maio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint 2</t>
   </si>
   <si>
+    <t>07-Maio</t>
+  </si>
+  <si>
+    <t>09-Maio</t>
+  </si>
+  <si>
+    <t>14-Maio</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;Sprint 2&lt;/strong&gt;</t>
   </si>
   <si>
+    <t>16-Maio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint 3</t>
   </si>
   <si>
+    <t>21-Maio</t>
+  </si>
+  <si>
+    <t>23-Maio</t>
+  </si>
+  <si>
+    <t>28-Maio</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;Sprint 3&lt;/strong&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 4&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 5&lt;/strong&gt;</t>
+    <t>30-Maio</t>
+  </si>
+  <si>
+    <t>Feriado</t>
+  </si>
+  <si>
+    <t>04-Junho</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Demo day&lt;/strong&gt;</t>
@@ -323,14 +416,14 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -846,7 +939,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -876,637 +969,631 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
+    <row r="4" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="49.5" customHeight="1">
+    <row r="5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
+    <row r="6" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
+    <row r="7" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>38</v>
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>41</v>
+    <row r="11" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>45</v>
+    <row r="12" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>48</v>
+    <row r="13" s="1" customFormat="1" ht="50.25" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>52</v>
+      <c r="A14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>55</v>
+    <row r="15" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
+    <row r="16" s="1" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A17" s="5">
-        <v>16</v>
+    <row r="17" s="1" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>61</v>
+      <c r="C17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A18" s="4">
-        <v>17</v>
+    <row r="18" s="1" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>67</v>
+    <row r="19" s="1" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>71</v>
+    <row r="20" s="1" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="56.25" customHeight="1">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>71</v>
+    <row r="21" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>71</v>
+    <row r="22" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>74</v>
+    <row r="23" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" s="1" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>71</v>
+    <row r="24" s="1" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="4">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="4">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>71</v>
+    <row r="25" s="1" customFormat="1" ht="44.25" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>74</v>
+    <row r="27" s="1" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>71</v>
+      <c r="A29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>71</v>
+      <c r="A30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5"/>
+      <c r="A31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>74</v>
+        <v>106</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="1"/>
+      <c r="A32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A33" s="5">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="1"/>
+      <c r="A33" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="4">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>71</v>
+      <c r="A35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" ht="28.5">
-      <c r="A37" s="6">
-        <v>36</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" ht="28.5">
-      <c r="A38" s="6">
-        <v>37</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>71</v>
-      </c>
+    <row r="37" ht="14.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="6">
-        <v>38</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="6">
-        <v>39</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
alteracoes pos conversa nakagawa
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Empreendedorismo é um comportamento para o desenvolvimento de pessoas, de organizações e do mundo; Aproveite as oportunidades que serão oferecidas no curso</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação da disciplina; Bate papo com empreendedores do Insper.</t>
+    <t xml:space="preserve">Apresentação da disciplina.</t>
   </si>
   <si>
     <t>8-Fev</t>
@@ -225,7 +225,7 @@
     <t>28-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">Avaliação intermediária - não teremos aula</t>
+    <t xml:space="preserve">Avaliação intermediária</t>
   </si>
   <si>
     <t>02-Abril</t>
@@ -939,7 +939,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
atualizacao plano de aula e referencias
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Data</t>
   </si>
@@ -201,31 +201,34 @@
     <t xml:space="preserve">Como desenvolver soluções de IA?</t>
   </si>
   <si>
-    <t xml:space="preserve">A solução imaginada é factível? Quais são os recursos necessários para o desenvolvimento da solução? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mapeamento modelo, fontes de informação e dados. Mapeamento da qualidade e disponibilidade dos dados. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercício que envolve a identificação das informações necessárias para o desenvolvimento da solução, mapeamento das fontes disponíveis de dados, da qualidade destas fontes e real disponibilidade. </t>
+    <t xml:space="preserve">A solução imaginada é factível? Quais são os recursos necessários para o desenvolvimento da solução? Qual o processo normalmente empregado no desenvolvimento de soluções de machine learning? CRISP-DM, KDD e reutilização de modelos e serviços.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapeamento modelo, fontes de informação e dados. Mapeamento da qualidade e disponibilidade dos dados. CRISP-DM, KDD, identificação de oportunidades para reutilização de modelos e utilização de serviços de IA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercício que envolve a identificação das informações necessárias para o desenvolvimento da solução, mapeamento das fontes disponíveis de dados, da qualidade destas fontes e real disponibilidade. Aula expositiva sobre os processos normalmente empregados no mercado e debate sobre como aplicar tais processos no desenvolvimento da solução de cada equipe.</t>
   </si>
   <si>
     <t>26-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">Qual o processo normalmente empregado no desenvolvimento de soluções de machine learning? CRISP-DM, KDD e reutilização de modelos e serviços</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRISP-DM, KDD, identificação de oportunidades para reutilização de modelos e utilização de serviços de IA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula expositiva sobre os processos normalmente empregados no mercado e debate sobre como aplicar tais processos no desenvolvimento da solução de cada equipe</t>
+    <t xml:space="preserve">Ética em IA. O que são soluções éticas e o que não são soluções éticas? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como desenvolver soluções baseadas em machine learning com princípios éticos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva sobre ética em IA seguido de debate sobre como aplicar tais conceitos no desenvolvimento da solução de cada equipe. </t>
   </si>
   <si>
     <t>28-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">Avaliação intermediária</t>
+    <t xml:space="preserve">&lt;strong&gt;Avaliação intermediária&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Avaliação intermediária. Apresentação dos projetos em andamento para o Centro de Empreendedorismo do Insper.&lt;/strong&gt;</t>
   </si>
   <si>
     <t>02-Abril</t>
@@ -234,118 +237,97 @@
     <t>04-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Produto Viável Mínimo (MVP). Por que usar este conceito? Como definir o seu MVP? A importância de um roadmap para a solução.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definição do MVP para cada solução. Elaboração inicial de um roadmap.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breve exposição sobre o conceito de MVP seguido por debate sobre a definição dos MVPs para cada solução. </t>
+    <t xml:space="preserve">Produto Viável Mínimo (MVP). Por que usar este conceito? Como definir o seu MVP? A importância de um roadmap para a solução. Infra-estrutura (github, nuvem). Processos de trabalho (branch, pull request). Testes automatizados, documentação e padronização de código.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição do MVP para cada solução. Elaboração inicial de um roadmap. Infra-estutura do projeto configurada e processos de trabalho definidos. Cada equipe deverá definir como os testes automatizados, documentação e padronização de código serão feitos no escopo dos seus projetos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breve exposição sobre o conceito de MVP seguido por debate sobre a definição dos MVPs para cada solução. Debate sobre o uso de github, serviços em nuvem e processos de trabalho. Breve exposição sobre a importância de testes automatizados, documentação e padronização de código no escopo de startups. Apresentação de ferramentas que podem auxiliar as equipes nestas tarefas. Discussão entre as equipes para definir os padrões e ferramentas que serão adotados em cada equipe. </t>
   </si>
   <si>
     <t>09-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Infra-estrutura (github, nuvem). Processos de trabalho (branch, pull request)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infra-estutura do projeto configurada e processos de trabalho definidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debate sobre o uso de github, serviços em nuvem e processos de trabalho.</t>
+    <t xml:space="preserve">Desenvolvimento da solução</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evolução do código gerado, do quadro de atividades, dos modelos de machine learning e das funcionalidades da solução.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento da solução.</t>
   </si>
   <si>
     <t>11-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Processos, MVP, infra-estrutura na prática</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As equipes souberam definir o seu MVP? Fizeram o mapeamento de dados necessários? Estão com a infra-estrutura configurada?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkpoint com todas as equipes para verificar os artefatos de projeto produzidos até o momento.</t>
-  </si>
-  <si>
     <t>16-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Testes automatizados, documentação e padronização de código</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cada equipe deverá definir como os testes automatizados, documentação e padronização de código serão feitos no escopo dos seus projetos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breve exposição sobre a importância de testes automatizados, documentação e padronização de código no escopo de startups. Apresentação de ferramentas que podem auxiliar as equipes nestas tarefas. Discussão entre as equipes para definir os padrões e ferramentas que serão adotados em cada equipe. </t>
-  </si>
-  <si>
     <t>18-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolvimento da solução</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evolução do código gerado, do quadro de atividades, dos modelos de machine learning e das funcionalidades da solução.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento da solução.</t>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 1&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Sprint review&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Apresentação e debate sobre as entregas do sprint.&lt;/strong&gt;</t>
   </si>
   <si>
     <t>23-Abril</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprint 2</t>
+  </si>
+  <si>
     <t>25-Abril</t>
   </si>
   <si>
     <t>30-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 1&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint review&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Apresentação e debate sobre as entregas do sprint.&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>02-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint 2</t>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 2&lt;/strong&gt;</t>
   </si>
   <si>
     <t>07-Maio</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprint 3</t>
+  </si>
+  <si>
     <t>09-Maio</t>
   </si>
   <si>
     <t>14-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 2&lt;/strong&gt;</t>
-  </si>
-  <si>
     <t>16-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint 3</t>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 3&lt;/strong&gt;</t>
   </si>
   <si>
     <t>21-Maio</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprint 4</t>
+  </si>
+  <si>
     <t>23-Maio</t>
   </si>
   <si>
     <t>28-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 3&lt;/strong&gt;</t>
+    <t xml:space="preserve">&lt;strong&gt;Sprint 4&lt;/strong&gt;</t>
   </si>
   <si>
     <t>30-Maio</t>
@@ -939,7 +921,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1212,13 +1194,13 @@
         <v>65</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="5" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="2"/>
@@ -1231,17 +1213,17 @@
       <c r="C17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>70</v>
+      <c r="E17" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="78.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="1" t="s">
@@ -1251,297 +1233,296 @@
         <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="63.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="45.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="41.25" customHeight="1">
       <c r="A21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="41.25" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="49.5" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="44.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>99</v>
+      <c r="A27" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>100</v>
+      <c r="C28" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>100</v>
+      <c r="C29" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="3" t="s">
-        <v>104</v>
+      <c r="C30" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>106</v>
+      <c r="C31" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F36" s="1"/>
     </row>

</xml_diff>

<commit_message>
pequena alteracao plano de aula
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Data</t>
   </si>
@@ -325,18 +325,6 @@
   </si>
   <si>
     <t>28-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Sprint 4&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>30-Maio</t>
-  </si>
-  <si>
-    <t>Feriado</t>
-  </si>
-  <si>
-    <t>04-Junho</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Demo day&lt;/strong&gt;</t>
@@ -390,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -403,9 +391,6 @@
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -921,7 +906,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -995,7 +980,7 @@
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1011,7 +996,9 @@
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1027,7 +1014,9 @@
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1043,7 +1032,9 @@
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1050,9 @@
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1077,7 +1070,9 @@
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1111,7 +1106,9 @@
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>45</v>
       </c>
@@ -1127,7 +1124,9 @@
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
@@ -1143,7 +1142,9 @@
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
@@ -1159,7 +1160,9 @@
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>57</v>
       </c>
@@ -1193,14 +1196,16 @@
       <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="2"/>
@@ -1209,14 +1214,16 @@
       <c r="A17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F17" s="2"/>
@@ -1225,7 +1232,9 @@
       <c r="A18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>70</v>
       </c>
@@ -1241,7 +1250,9 @@
       <c r="A19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>74</v>
       </c>
@@ -1275,7 +1286,9 @@
       <c r="A21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>79</v>
       </c>
@@ -1291,7 +1304,9 @@
       <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>79</v>
       </c>
@@ -1307,6 +1322,9 @@
       <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>85</v>
       </c>
@@ -1322,7 +1340,9 @@
       <c r="A24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>89</v>
       </c>
@@ -1338,7 +1358,9 @@
       <c r="A25" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>89</v>
       </c>
@@ -1354,7 +1376,9 @@
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C26" s="3" t="s">
         <v>89</v>
       </c>
@@ -1370,7 +1394,9 @@
       <c r="A27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>93</v>
       </c>
@@ -1386,7 +1412,9 @@
       <c r="A28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>95</v>
       </c>
@@ -1402,7 +1430,9 @@
       <c r="A29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>95</v>
       </c>
@@ -1418,7 +1448,9 @@
       <c r="A30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>95</v>
       </c>
@@ -1434,7 +1466,9 @@
       <c r="A31" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>99</v>
       </c>
@@ -1450,7 +1484,9 @@
       <c r="A32" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>101</v>
       </c>
@@ -1466,7 +1502,9 @@
       <c r="A33" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>101</v>
       </c>
@@ -1482,53 +1520,36 @@
       <c r="A34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>87</v>
+      <c r="D34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="6" t="s">
-        <v>107</v>
-      </c>
+      <c r="A36" s="5"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>

</xml_diff>